<commit_message>
made graphs for exp 1 and most of exp 2 and added them to latex
</commit_message>
<xml_diff>
--- a/lab3/Experiment 1/bjtWithIc .xlsx
+++ b/lab3/Experiment 1/bjtWithIc .xlsx
@@ -10,7 +10,6 @@
     <sheet name="bjtWithIc" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="145621"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -609,7 +608,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Base/Current</a:t>
+              <a:t>Base/Collector</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
@@ -3022,11 +3021,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="65650688"/>
-        <c:axId val="65651264"/>
+        <c:axId val="94637440"/>
+        <c:axId val="94635136"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="65650688"/>
+        <c:axId val="94637440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.37500000000000006"/>
@@ -3066,12 +3065,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="65651264"/>
+        <c:crossAx val="94635136"/>
         <c:crossesAt val="1.0000000000000005E-8"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="65651264"/>
+        <c:axId val="94635136"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -3113,7 +3112,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="65650688"/>
+        <c:crossAx val="94637440"/>
         <c:crossesAt val="0.37500000000000006"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3178,6 +3177,11 @@
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
@@ -3913,11 +3917,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="65653568"/>
-        <c:axId val="65654144"/>
+        <c:axId val="94639744"/>
+        <c:axId val="94640320"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="65653568"/>
+        <c:axId val="94639744"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -3958,12 +3962,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="65654144"/>
+        <c:crossAx val="94640320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="65654144"/>
+        <c:axId val="94640320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="11"/>
@@ -4005,7 +4009,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="65653568"/>
+        <c:crossAx val="94639744"/>
         <c:crossesAt val="1.0000000000000005E-8"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4041,6 +4045,11 @@
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
@@ -4753,11 +4762,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="65655872"/>
-        <c:axId val="65656448"/>
+        <c:axId val="114278400"/>
+        <c:axId val="114278976"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="65655872"/>
+        <c:axId val="114278400"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -4798,12 +4807,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="65656448"/>
+        <c:crossAx val="114278976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="65656448"/>
+        <c:axId val="114278976"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -4852,7 +4861,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="65655872"/>
+        <c:crossAx val="114278400"/>
         <c:crossesAt val="1.0000000000000005E-8"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4892,6 +4901,11 @@
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
@@ -5603,11 +5617,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="65658176"/>
-        <c:axId val="44965888"/>
+        <c:axId val="114280704"/>
+        <c:axId val="114281280"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="65658176"/>
+        <c:axId val="114280704"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -5616,6 +5630,21 @@
         <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1600"/>
+                  <a:t>Base Current</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
           <c:layout/>
           <c:overlay val="0"/>
         </c:title>
@@ -5633,12 +5662,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="44965888"/>
+        <c:crossAx val="114281280"/>
         <c:crossesAt val="1.0000000000000004E-6"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="44965888"/>
+        <c:axId val="114281280"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -5647,6 +5676,21 @@
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1600"/>
+                  <a:t>Transductance Gain</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
           <c:layout/>
           <c:overlay val="0"/>
         </c:title>
@@ -5664,7 +5708,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="65658176"/>
+        <c:crossAx val="114280704"/>
         <c:crossesAt val="1.0000000000000005E-7"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5701,6 +5745,11 @@
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
@@ -6123,7 +6172,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
       <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added stuff from lab3
</commit_message>
<xml_diff>
--- a/lab3/Experiment 1/bjtWithIc .xlsx
+++ b/lab3/Experiment 1/bjtWithIc .xlsx
@@ -631,7 +631,7 @@
           <c:x val="0.1508198878240995"/>
           <c:y val="0.10585549447828456"/>
           <c:w val="0.79377471226949348"/>
-          <c:h val="0.78933002784312067"/>
+          <c:h val="0.76584664605006991"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -1948,36 +1948,26 @@
               </a:ln>
             </c:spPr>
             <c:trendlineType val="exp"/>
-            <c:dispRSqr val="0"/>
+            <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.13725989677646883"/>
-                  <c:y val="0.39269881068086526"/>
+                  <c:x val="-0.11486540926570225"/>
+                  <c:y val="0.39213837984026595"/>
                 </c:manualLayout>
               </c:layout>
-              <c:tx>
-                <c:rich>
-                  <a:bodyPr/>
-                  <a:lstStyle/>
-                  <a:p>
-                    <a:pPr>
-                      <a:defRPr/>
-                    </a:pPr>
-                    <a:r>
-                      <a:rPr lang="en-US" sz="1600" baseline="0"/>
-                      <a:t>y = 1E-14e</a:t>
-                    </a:r>
-                    <a:r>
-                      <a:rPr lang="en-US" sz="1600" baseline="30000"/>
-                      <a:t>36.974x</a:t>
-                    </a:r>
-                    <a:endParaRPr lang="en-US" sz="1600"/>
-                  </a:p>
-                </c:rich>
-              </c:tx>
               <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:txPr>
+                <a:bodyPr/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr/>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
             </c:trendlineLbl>
           </c:trendline>
           <c:xVal>
@@ -2496,36 +2486,26 @@
               </a:ln>
             </c:spPr>
             <c:trendlineType val="exp"/>
-            <c:dispRSqr val="0"/>
+            <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.12692397946380735"/>
-                  <c:y val="2.7716347621126965E-2"/>
+                  <c:x val="-0.14380043857620031"/>
+                  <c:y val="-1.4850195468676935E-3"/>
                 </c:manualLayout>
               </c:layout>
-              <c:tx>
-                <c:rich>
-                  <a:bodyPr/>
-                  <a:lstStyle/>
-                  <a:p>
-                    <a:pPr>
-                      <a:defRPr/>
-                    </a:pPr>
-                    <a:r>
-                      <a:rPr lang="en-US" sz="1600" baseline="0"/>
-                      <a:t>y = 3E-14e</a:t>
-                    </a:r>
-                    <a:r>
-                      <a:rPr lang="en-US" sz="1600" baseline="30000"/>
-                      <a:t>38.051x</a:t>
-                    </a:r>
-                    <a:endParaRPr lang="en-US" sz="1600"/>
-                  </a:p>
-                </c:rich>
-              </c:tx>
               <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:txPr>
+                <a:bodyPr/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr/>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
             </c:trendlineLbl>
           </c:trendline>
           <c:xVal>
@@ -3021,11 +3001,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="94637440"/>
-        <c:axId val="94635136"/>
+        <c:axId val="113459776"/>
+        <c:axId val="113460352"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="94637440"/>
+        <c:axId val="113459776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.37500000000000006"/>
@@ -3065,12 +3045,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="94635136"/>
+        <c:crossAx val="113460352"/>
         <c:crossesAt val="1.0000000000000005E-8"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="94635136"/>
+        <c:axId val="113460352"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -3112,7 +3092,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="94637440"/>
+        <c:crossAx val="113459776"/>
         <c:crossesAt val="0.37500000000000006"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3917,11 +3897,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="94639744"/>
-        <c:axId val="94640320"/>
+        <c:axId val="113462656"/>
+        <c:axId val="113463232"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="94639744"/>
+        <c:axId val="113462656"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -3962,12 +3942,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="94640320"/>
+        <c:crossAx val="113463232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="94640320"/>
+        <c:axId val="113463232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="11"/>
@@ -4009,7 +3989,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="94639744"/>
+        <c:crossAx val="113462656"/>
         <c:crossesAt val="1.0000000000000005E-8"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4121,7 +4101,7 @@
           </c:marker>
           <c:trendline>
             <c:trendlineType val="power"/>
-            <c:dispRSqr val="0"/>
+            <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
               <c:layout>
@@ -4762,11 +4742,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="114278400"/>
-        <c:axId val="114278976"/>
+        <c:axId val="113464960"/>
+        <c:axId val="113465536"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="114278400"/>
+        <c:axId val="113464960"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -4807,12 +4787,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="114278976"/>
+        <c:crossAx val="113465536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="114278976"/>
+        <c:axId val="113465536"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -4861,7 +4841,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="114278400"/>
+        <c:crossAx val="113464960"/>
         <c:crossesAt val="1.0000000000000005E-8"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4929,6 +4909,21 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Incremental Transductance Gain</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
     </c:title>
@@ -4976,13 +4971,13 @@
           </c:marker>
           <c:trendline>
             <c:trendlineType val="power"/>
-            <c:dispRSqr val="0"/>
+            <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.15388376840491838"/>
-                  <c:y val="5.9534164970951667E-2"/>
+                  <c:x val="-0.17127401710445109"/>
+                  <c:y val="7.7474180895927336E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -5617,11 +5612,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="114280704"/>
-        <c:axId val="114281280"/>
+        <c:axId val="117800960"/>
+        <c:axId val="117801536"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="114280704"/>
+        <c:axId val="117800960"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -5662,12 +5657,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="114281280"/>
+        <c:crossAx val="117801536"/>
         <c:crossesAt val="1.0000000000000004E-6"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="114281280"/>
+        <c:axId val="117801536"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -5684,6 +5679,14 @@
                 <a:pPr>
                   <a:defRPr/>
                 </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1600"/>
+                  <a:t>Incremental</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1600" baseline="0"/>
+                  <a:t> </a:t>
+                </a:r>
                 <a:r>
                   <a:rPr lang="en-US" sz="1600"/>
                   <a:t>Transductance Gain</a:t>
@@ -5708,7 +5711,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="114280704"/>
+        <c:crossAx val="117800960"/>
         <c:crossesAt val="1.0000000000000005E-7"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5762,16 +5765,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1114425</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>85724</xdr:rowOff>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
       <xdr:colOff>66675</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>76199</xdr:rowOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6172,8 +6175,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" topLeftCell="C76" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update lab 3 - revise report, add units to all graphs.
</commit_message>
<xml_diff>
--- a/lab3/Experiment 1/bjtWithIc .xlsx
+++ b/lab3/Experiment 1/bjtWithIc .xlsx
@@ -1957,17 +1957,32 @@
                   <c:y val="0.39213837984026595"/>
                 </c:manualLayout>
               </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr>
+                      <a:defRPr/>
+                    </a:pPr>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:t>y (A) = 1E-14e</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="30000"/>
+                      <a:t>36.974x (V)</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:t>
+R² = 0.9997</a:t>
+                    </a:r>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
               <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:txPr>
-                <a:bodyPr/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr/>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
             </c:trendlineLbl>
           </c:trendline>
           <c:xVal>
@@ -2495,17 +2510,32 @@
                   <c:y val="-1.4850195468676935E-3"/>
                 </c:manualLayout>
               </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr>
+                      <a:defRPr/>
+                    </a:pPr>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:t>y (A) = 3E-14e</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="30000"/>
+                      <a:t>38.051x (V)</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:t>
+R² = 0.9999</a:t>
+                    </a:r>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
               <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:txPr>
-                <a:bodyPr/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr/>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
             </c:trendlineLbl>
           </c:trendline>
           <c:xVal>
@@ -3001,11 +3031,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="113459776"/>
-        <c:axId val="113460352"/>
+        <c:axId val="524152192"/>
+        <c:axId val="522646592"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="113459776"/>
+        <c:axId val="524152192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.37500000000000006"/>
@@ -3023,7 +3053,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US" sz="1800"/>
-                  <a:t>Base Voltage</a:t>
+                  <a:t>Base Voltage (V)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -3045,12 +3075,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="113460352"/>
+        <c:crossAx val="522646592"/>
         <c:crossesAt val="1.0000000000000005E-8"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="113460352"/>
+        <c:axId val="522646592"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -3070,7 +3100,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US" sz="1800"/>
-                  <a:t>Base Current, Collector Current</a:t>
+                  <a:t>Base Current, Collector Current (A)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -3092,7 +3122,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="113459776"/>
+        <c:crossAx val="524152192"/>
         <c:crossesAt val="0.37500000000000006"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3897,11 +3927,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="113462656"/>
-        <c:axId val="113463232"/>
+        <c:axId val="511726080"/>
+        <c:axId val="511726656"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="113462656"/>
+        <c:axId val="511726080"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -3920,7 +3950,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US" sz="1800"/>
-                  <a:t>Base Current</a:t>
+                  <a:t>Base Current (A)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -3942,12 +3972,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="113463232"/>
+        <c:crossAx val="511726656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="113463232"/>
+        <c:axId val="511726656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="11"/>
@@ -3967,7 +3997,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US" sz="1800"/>
-                  <a:t>Beta</a:t>
+                  <a:t>Current Gain Beta</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -3989,7 +4019,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="113462656"/>
+        <c:crossAx val="511726080"/>
         <c:crossesAt val="1.0000000000000005E-8"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4110,17 +4140,38 @@
                   <c:y val="-0.56504797194468337"/>
                 </c:manualLayout>
               </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr>
+                      <a:defRPr sz="1600"/>
+                    </a:pPr>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:t>y = 0.0653x</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1600" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                        <a:effectLst/>
+                      </a:rPr>
+                      <a:t>(A)</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="30000"/>
+                      <a:t>-0.945 </a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:t>
+R² = 0.9973</a:t>
+                    </a:r>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
               <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:txPr>
-                <a:bodyPr/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="1600"/>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
             </c:trendlineLbl>
           </c:trendline>
           <c:xVal>
@@ -4742,11 +4793,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="113464960"/>
-        <c:axId val="113465536"/>
+        <c:axId val="511728384"/>
+        <c:axId val="511728960"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="113464960"/>
+        <c:axId val="511728384"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -4765,7 +4816,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US" sz="1600"/>
-                  <a:t>Base Current</a:t>
+                  <a:t>Base Current (A)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -4787,12 +4838,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="113465536"/>
+        <c:crossAx val="511728960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="113465536"/>
+        <c:axId val="511728960"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -4812,7 +4863,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US" sz="1800"/>
-                  <a:t>Incremental Resistance</a:t>
+                  <a:t>Incremental Resistance (Ohms)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -4841,7 +4892,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="113464960"/>
+        <c:crossAx val="511728384"/>
         <c:crossesAt val="1.0000000000000005E-8"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4980,17 +5031,32 @@
                   <c:y val="7.7474180895927336E-2"/>
                 </c:manualLayout>
               </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr>
+                      <a:defRPr sz="1400"/>
+                    </a:pPr>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:t>y = 23.009x(A)</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="30000"/>
+                      <a:t>0.9658</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:t>
+R² = 0.999</a:t>
+                    </a:r>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
               <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:txPr>
-                <a:bodyPr/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="1400"/>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
             </c:trendlineLbl>
           </c:trendline>
           <c:xVal>
@@ -5612,11 +5678,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="117800960"/>
-        <c:axId val="117801536"/>
+        <c:axId val="522642560"/>
+        <c:axId val="522643136"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="117800960"/>
+        <c:axId val="522642560"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -5635,7 +5701,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US" sz="1600"/>
-                  <a:t>Base Current</a:t>
+                  <a:t>Base Current (A)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -5657,12 +5723,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="117801536"/>
+        <c:crossAx val="522643136"/>
         <c:crossesAt val="1.0000000000000004E-6"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="117801536"/>
+        <c:axId val="522643136"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -5689,7 +5755,7 @@
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-US" sz="1600"/>
-                  <a:t>Transductance Gain</a:t>
+                  <a:t>Transductance Gain (Mhos)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -5711,7 +5777,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="117800960"/>
+        <c:crossAx val="522642560"/>
         <c:crossesAt val="1.0000000000000005E-7"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6175,8 +6241,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C76" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+    <sheetView tabSelected="1" topLeftCell="I52" workbookViewId="0">
+      <selection activeCell="I95" sqref="I95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>